<commit_message>
Culling fix + Central overheat stun + rotating gatti prefab
</commit_message>
<xml_diff>
--- a/Design/MechanicDesign.xlsx
+++ b/Design/MechanicDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="198">
   <si>
     <t>Range</t>
   </si>
@@ -562,9 +562,6 @@
     <t>minimap</t>
   </si>
   <si>
-    <t>hull health</t>
-  </si>
-  <si>
     <t>melee damage</t>
   </si>
   <si>
@@ -613,10 +610,16 @@
     <t>RADIATOR</t>
   </si>
   <si>
-    <t>central overheat limi</t>
+    <t>value</t>
   </si>
   <si>
-    <t>value</t>
+    <t>damage protection</t>
+  </si>
+  <si>
+    <t>hull overheat limi</t>
+  </si>
+  <si>
+    <t>hull armor</t>
   </si>
 </sst>
 </file>
@@ -1307,11 +1310,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66835200"/>
-        <c:axId val="66836736"/>
+        <c:axId val="116219904"/>
+        <c:axId val="116221440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66835200"/>
+        <c:axId val="116219904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1323,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66836736"/>
+        <c:crossAx val="116221440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1328,7 +1331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66836736"/>
+        <c:axId val="116221440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66835200"/>
+        <c:crossAx val="116219904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1449,11 +1452,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="189957248"/>
-        <c:axId val="189958784"/>
+        <c:axId val="126800256"/>
+        <c:axId val="126801792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189957248"/>
+        <c:axId val="126800256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +1465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189958784"/>
+        <c:crossAx val="126801792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1470,7 +1473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189958784"/>
+        <c:axId val="126801792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189957248"/>
+        <c:crossAx val="126800256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1597,11 +1600,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="189966976"/>
-        <c:axId val="189968768"/>
+        <c:axId val="126498688"/>
+        <c:axId val="126500224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189966976"/>
+        <c:axId val="126498688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189968768"/>
+        <c:crossAx val="126500224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1618,7 +1621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189968768"/>
+        <c:axId val="126500224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189966976"/>
+        <c:crossAx val="126498688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1700,7 +1703,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>hull health</c:v>
+                  <c:v>damage protection</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1713,19 +1716,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1740,11 +1743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190337408"/>
-        <c:axId val="190338944"/>
+        <c:axId val="126516608"/>
+        <c:axId val="126538880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190337408"/>
+        <c:axId val="126516608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190338944"/>
+        <c:crossAx val="126538880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1761,7 +1764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190338944"/>
+        <c:axId val="126538880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190337408"/>
+        <c:crossAx val="126516608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1883,11 +1886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190363520"/>
-        <c:axId val="190365056"/>
+        <c:axId val="126628992"/>
+        <c:axId val="126630528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190363520"/>
+        <c:axId val="126628992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190365056"/>
+        <c:crossAx val="126630528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1904,7 +1907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190365056"/>
+        <c:axId val="126630528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,7 +1918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190363520"/>
+        <c:crossAx val="126628992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2026,11 +2029,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="190389632"/>
-        <c:axId val="190395520"/>
+        <c:axId val="126651008"/>
+        <c:axId val="126652800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190389632"/>
+        <c:axId val="126651008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,7 +2042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190395520"/>
+        <c:crossAx val="126652800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2047,7 +2050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190395520"/>
+        <c:axId val="126652800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2058,7 +2061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190389632"/>
+        <c:crossAx val="126651008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2516,11 +2519,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="79985664"/>
-        <c:axId val="79995648"/>
+        <c:axId val="127162624"/>
+        <c:axId val="125243392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79985664"/>
+        <c:axId val="127162624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2529,7 +2532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79995648"/>
+        <c:crossAx val="125243392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2537,7 +2540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79995648"/>
+        <c:axId val="125243392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,7 +2551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79985664"/>
+        <c:crossAx val="127162624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3005,11 +3008,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80106624"/>
-        <c:axId val="80108160"/>
+        <c:axId val="125276544"/>
+        <c:axId val="125278080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80106624"/>
+        <c:axId val="125276544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3018,7 +3021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80108160"/>
+        <c:crossAx val="125278080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3026,7 +3029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80108160"/>
+        <c:axId val="125278080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80106624"/>
+        <c:crossAx val="125276544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3494,11 +3497,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80133120"/>
-        <c:axId val="66913024"/>
+        <c:axId val="127342848"/>
+        <c:axId val="127361024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80133120"/>
+        <c:axId val="127342848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3507,7 +3510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66913024"/>
+        <c:crossAx val="127361024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3515,7 +3518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66913024"/>
+        <c:axId val="127361024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3526,7 +3529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80133120"/>
+        <c:crossAx val="127342848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3983,11 +3986,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66942080"/>
-        <c:axId val="66943616"/>
+        <c:axId val="127385984"/>
+        <c:axId val="127387520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66942080"/>
+        <c:axId val="127385984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3996,7 +3999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66943616"/>
+        <c:crossAx val="127387520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4004,7 +4007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66943616"/>
+        <c:axId val="127387520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4015,7 +4018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66942080"/>
+        <c:crossAx val="127385984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4472,11 +4475,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67116032"/>
-        <c:axId val="67126016"/>
+        <c:axId val="127494400"/>
+        <c:axId val="127504384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67116032"/>
+        <c:axId val="127494400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4485,7 +4488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67126016"/>
+        <c:crossAx val="127504384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4493,7 +4496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67126016"/>
+        <c:axId val="127504384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4504,7 +4507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67116032"/>
+        <c:crossAx val="127494400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4979,11 +4982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="77610368"/>
-        <c:axId val="77612160"/>
+        <c:axId val="116300416"/>
+        <c:axId val="116306304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77610368"/>
+        <c:axId val="116300416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4992,7 +4995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77612160"/>
+        <c:crossAx val="116306304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5000,7 +5003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77612160"/>
+        <c:axId val="116306304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5013,7 +5016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77610368"/>
+        <c:crossAx val="116300416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5470,11 +5473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67167360"/>
-        <c:axId val="67168896"/>
+        <c:axId val="127541632"/>
+        <c:axId val="127543168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67167360"/>
+        <c:axId val="127541632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5483,7 +5486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67168896"/>
+        <c:crossAx val="127543168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5491,7 +5494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67168896"/>
+        <c:axId val="127543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5502,7 +5505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67167360"/>
+        <c:crossAx val="127541632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5959,11 +5962,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80456704"/>
-        <c:axId val="80462592"/>
+        <c:axId val="127588608"/>
+        <c:axId val="127594496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80456704"/>
+        <c:axId val="127588608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5972,7 +5975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80462592"/>
+        <c:crossAx val="127594496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5980,7 +5983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80462592"/>
+        <c:axId val="127594496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5991,7 +5994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80456704"/>
+        <c:crossAx val="127588608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6448,11 +6451,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80491648"/>
-        <c:axId val="80493184"/>
+        <c:axId val="127639936"/>
+        <c:axId val="127641472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80491648"/>
+        <c:axId val="127639936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6461,7 +6464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80493184"/>
+        <c:crossAx val="127641472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6469,7 +6472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80493184"/>
+        <c:axId val="127641472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6480,7 +6483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80491648"/>
+        <c:crossAx val="127639936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6937,11 +6940,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80616448"/>
-        <c:axId val="80622336"/>
+        <c:axId val="128010496"/>
+        <c:axId val="128016384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80616448"/>
+        <c:axId val="128010496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6950,7 +6953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80622336"/>
+        <c:crossAx val="128016384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6958,7 +6961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80622336"/>
+        <c:axId val="128016384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6969,7 +6972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80616448"/>
+        <c:crossAx val="128010496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7111,11 +7114,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80646912"/>
-        <c:axId val="80648448"/>
+        <c:axId val="125419520"/>
+        <c:axId val="125421056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80646912"/>
+        <c:axId val="125419520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7125,7 +7128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80648448"/>
+        <c:crossAx val="125421056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7135,7 +7138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80648448"/>
+        <c:axId val="125421056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7148,7 +7151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80646912"/>
+        <c:crossAx val="125419520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7605,11 +7608,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80888960"/>
-        <c:axId val="80890496"/>
+        <c:axId val="127910272"/>
+        <c:axId val="127911808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80888960"/>
+        <c:axId val="127910272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7618,7 +7621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80890496"/>
+        <c:crossAx val="127911808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7626,7 +7629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80890496"/>
+        <c:axId val="127911808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7637,7 +7640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80888960"/>
+        <c:crossAx val="127910272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7838,11 +7841,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80918016"/>
-        <c:axId val="80926592"/>
+        <c:axId val="128042880"/>
+        <c:axId val="127935616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80918016"/>
+        <c:axId val="128042880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7851,7 +7854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80926592"/>
+        <c:crossAx val="127935616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7859,7 +7862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80926592"/>
+        <c:axId val="127935616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7870,7 +7873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80918016"/>
+        <c:crossAx val="128042880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8015,11 +8018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="51190016"/>
-        <c:axId val="51195904"/>
+        <c:axId val="129660416"/>
+        <c:axId val="129661952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51190016"/>
+        <c:axId val="129660416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8028,7 +8031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51195904"/>
+        <c:crossAx val="129661952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8036,7 +8039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51195904"/>
+        <c:axId val="129661952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8047,7 +8050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51190016"/>
+        <c:crossAx val="129660416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8145,11 +8148,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81278464"/>
-        <c:axId val="81280000"/>
+        <c:axId val="129532672"/>
+        <c:axId val="129534208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81278464"/>
+        <c:axId val="129532672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8158,7 +8161,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81280000"/>
+        <c:crossAx val="129534208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8166,7 +8169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81280000"/>
+        <c:axId val="129534208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8177,13 +8180,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81278464"/>
+        <c:crossAx val="129532672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8402,11 +8406,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81326464"/>
-        <c:axId val="81328000"/>
+        <c:axId val="129416576"/>
+        <c:axId val="129418368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81326464"/>
+        <c:axId val="129416576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8415,7 +8419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81328000"/>
+        <c:crossAx val="129418368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8423,7 +8427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81328000"/>
+        <c:axId val="129418368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8434,13 +8438,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81326464"/>
+        <c:crossAx val="129416576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8909,11 +8914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="188966784"/>
-        <c:axId val="188968320"/>
+        <c:axId val="126022784"/>
+        <c:axId val="126024320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="188966784"/>
+        <c:axId val="126022784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8922,7 +8927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188968320"/>
+        <c:crossAx val="126024320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8930,7 +8935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188968320"/>
+        <c:axId val="126024320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -8943,7 +8948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188966784"/>
+        <c:crossAx val="126022784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9094,11 +9099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81213696"/>
-        <c:axId val="81223680"/>
+        <c:axId val="130225664"/>
+        <c:axId val="130227200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81213696"/>
+        <c:axId val="130225664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9107,7 +9112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81223680"/>
+        <c:crossAx val="130227200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9115,7 +9120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81223680"/>
+        <c:axId val="130227200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9126,13 +9131,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81213696"/>
+        <c:crossAx val="130225664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9238,11 +9244,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81231232"/>
-        <c:axId val="81249408"/>
+        <c:axId val="130239104"/>
+        <c:axId val="130249088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81231232"/>
+        <c:axId val="130239104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9251,7 +9257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81249408"/>
+        <c:crossAx val="130249088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9259,7 +9265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81249408"/>
+        <c:axId val="130249088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9270,7 +9276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81231232"/>
+        <c:crossAx val="130239104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9471,11 +9477,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81986688"/>
-        <c:axId val="82007168"/>
+        <c:axId val="130271872"/>
+        <c:axId val="129843584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81986688"/>
+        <c:axId val="130271872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9484,7 +9490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82007168"/>
+        <c:crossAx val="129843584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9492,7 +9498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82007168"/>
+        <c:axId val="129843584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9503,7 +9509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81986688"/>
+        <c:crossAx val="130271872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9670,11 +9676,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81167872"/>
-        <c:axId val="81169408"/>
+        <c:axId val="129872640"/>
+        <c:axId val="129874176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81167872"/>
+        <c:axId val="129872640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9683,7 +9689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81169408"/>
+        <c:crossAx val="129874176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9691,7 +9697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81169408"/>
+        <c:axId val="129874176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9702,7 +9708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81167872"/>
+        <c:crossAx val="129872640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9869,11 +9875,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81190272"/>
-        <c:axId val="81196160"/>
+        <c:axId val="130042496"/>
+        <c:axId val="130044288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81190272"/>
+        <c:axId val="130042496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9882,7 +9888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81196160"/>
+        <c:crossAx val="130044288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9890,7 +9896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81196160"/>
+        <c:axId val="130044288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9901,7 +9907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81190272"/>
+        <c:crossAx val="130042496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10068,11 +10074,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81880576"/>
-        <c:axId val="81882112"/>
+        <c:axId val="130069248"/>
+        <c:axId val="130070784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81880576"/>
+        <c:axId val="130069248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10081,7 +10087,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81882112"/>
+        <c:crossAx val="130070784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10089,7 +10095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81882112"/>
+        <c:axId val="130070784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10100,7 +10106,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81880576"/>
+        <c:crossAx val="130069248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10267,11 +10273,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82324864"/>
-        <c:axId val="82359424"/>
+        <c:axId val="130079360"/>
+        <c:axId val="130175360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82324864"/>
+        <c:axId val="130079360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10280,7 +10286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82359424"/>
+        <c:crossAx val="130175360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10288,7 +10294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82359424"/>
+        <c:axId val="130175360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10299,7 +10305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82324864"/>
+        <c:crossAx val="130079360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10466,11 +10472,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82380288"/>
-        <c:axId val="82381824"/>
+        <c:axId val="130208512"/>
+        <c:axId val="130210048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82380288"/>
+        <c:axId val="130208512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10479,7 +10485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82381824"/>
+        <c:crossAx val="130210048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10487,7 +10493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82381824"/>
+        <c:axId val="130210048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10498,7 +10504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82380288"/>
+        <c:crossAx val="130208512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10665,11 +10671,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82402688"/>
-        <c:axId val="82412672"/>
+        <c:axId val="130632320"/>
+        <c:axId val="130642304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82402688"/>
+        <c:axId val="130632320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10678,7 +10684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82412672"/>
+        <c:crossAx val="130642304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10686,7 +10692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82412672"/>
+        <c:axId val="130642304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10697,7 +10703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82402688"/>
+        <c:crossAx val="130632320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11172,11 +11178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189228928"/>
-        <c:axId val="189230464"/>
+        <c:axId val="126066048"/>
+        <c:axId val="126071936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189228928"/>
+        <c:axId val="126066048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11185,7 +11191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189230464"/>
+        <c:crossAx val="126071936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11193,7 +11199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189230464"/>
+        <c:axId val="126071936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11206,7 +11212,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189228928"/>
+        <c:crossAx val="126066048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11681,11 +11687,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189367040"/>
-        <c:axId val="189368576"/>
+        <c:axId val="126184832"/>
+        <c:axId val="126198912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189367040"/>
+        <c:axId val="126184832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11694,7 +11700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189368576"/>
+        <c:crossAx val="126198912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11702,7 +11708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189368576"/>
+        <c:axId val="126198912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11715,7 +11721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189367040"/>
+        <c:crossAx val="126184832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11766,7 +11772,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12191,11 +12196,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189418880"/>
-        <c:axId val="189432960"/>
+        <c:axId val="126261888"/>
+        <c:axId val="126267776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189418880"/>
+        <c:axId val="126261888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12204,7 +12209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189432960"/>
+        <c:crossAx val="126267776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12212,7 +12217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189432960"/>
+        <c:axId val="126267776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -12225,14 +12230,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189418880"/>
+        <c:crossAx val="126261888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12702,11 +12706,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189765504"/>
-        <c:axId val="189767040"/>
+        <c:axId val="126389632"/>
+        <c:axId val="126391424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189765504"/>
+        <c:axId val="126389632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12715,7 +12719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189767040"/>
+        <c:crossAx val="126391424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12723,7 +12727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189767040"/>
+        <c:axId val="126391424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -12736,7 +12740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189765504"/>
+        <c:crossAx val="126389632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13213,11 +13217,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189892864"/>
-        <c:axId val="189898752"/>
+        <c:axId val="126453248"/>
+        <c:axId val="126454784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189892864"/>
+        <c:axId val="126453248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13226,7 +13230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189898752"/>
+        <c:crossAx val="126454784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13234,7 +13238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189898752"/>
+        <c:axId val="126454784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -13247,7 +13251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189892864"/>
+        <c:crossAx val="126453248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13358,11 +13362,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="189910400"/>
-        <c:axId val="189920384"/>
+        <c:axId val="126757504"/>
+        <c:axId val="126763392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189910400"/>
+        <c:axId val="126757504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13371,7 +13375,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189920384"/>
+        <c:crossAx val="126763392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13379,7 +13383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189920384"/>
+        <c:axId val="126763392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13390,7 +13394,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189910400"/>
+        <c:crossAx val="126757504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13525,11 +13529,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$L$202" horiz="1" max="100" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$L$202" horiz="1" max="100" page="10"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$L$204" horiz="1" max="100" page="10" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$L$204" horiz="1" max="100" page="10" val="20"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24407,8 +24411,8 @@
     <tableColumn id="2" name="mark"/>
     <tableColumn id="3" name="radar radius"/>
     <tableColumn id="4" name="accuracy"/>
-    <tableColumn id="5" name="central overheat limi"/>
-    <tableColumn id="6" name="hull health"/>
+    <tableColumn id="5" name="hull overheat limi"/>
+    <tableColumn id="6" name="hull armor"/>
     <tableColumn id="7" name="melee damage"/>
     <tableColumn id="8" name="cooling rate"/>
     <tableColumn id="9" name="minimap"/>
@@ -24898,8 +24902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24948,7 +24952,7 @@
         <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L2" t="s">
         <v>153</v>
@@ -24957,13 +24961,13 @@
         <v>110</v>
       </c>
       <c r="N2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O2" t="s">
         <v>187</v>
       </c>
-      <c r="O2" t="s">
-        <v>188</v>
-      </c>
       <c r="P2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q2" t="s">
         <v>136</v>
@@ -25462,13 +25466,13 @@
         <v>43</v>
       </c>
       <c r="P14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="Q14" t="s">
+        <v>197</v>
+      </c>
+      <c r="R14" t="s">
         <v>178</v>
-      </c>
-      <c r="R14" t="s">
-        <v>179</v>
       </c>
       <c r="S14" t="s">
         <v>90</v>
@@ -26210,7 +26214,7 @@
       </c>
       <c r="Q30">
         <f>'ITEM STATS'!L209</f>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -26256,7 +26260,7 @@
       </c>
       <c r="Q31">
         <f>'ITEM STATS'!L210</f>
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -26302,7 +26306,7 @@
       </c>
       <c r="Q32">
         <f>'ITEM STATS'!L211</f>
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -26348,7 +26352,7 @@
       </c>
       <c r="Q33">
         <f>'ITEM STATS'!L212</f>
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -26394,7 +26398,7 @@
       </c>
       <c r="Q34">
         <f>'ITEM STATS'!L213</f>
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -26663,7 +26667,7 @@
         <v>40</v>
       </c>
       <c r="L40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M40">
         <v>1</v>
@@ -26709,7 +26713,7 @@
         <v>40</v>
       </c>
       <c r="L41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M41">
         <v>2</v>
@@ -26755,7 +26759,7 @@
         <v>40</v>
       </c>
       <c r="L42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M42">
         <v>3</v>
@@ -26801,7 +26805,7 @@
         <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M43">
         <v>4</v>
@@ -26847,7 +26851,7 @@
         <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M44">
         <v>5</v>
@@ -32930,8 +32934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:N228"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="L209" sqref="L209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33525,7 +33529,7 @@
         <v>46</v>
       </c>
       <c r="I36" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -33644,7 +33648,7 @@
         <v>46</v>
       </c>
       <c r="I43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -34021,7 +34025,7 @@
         <v>46</v>
       </c>
       <c r="I57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -34140,7 +34144,7 @@
         <v>46</v>
       </c>
       <c r="I64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -34517,7 +34521,7 @@
         <v>46</v>
       </c>
       <c r="I78" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -34636,7 +34640,7 @@
         <v>46</v>
       </c>
       <c r="I85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -35013,7 +35017,7 @@
         <v>46</v>
       </c>
       <c r="I99" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -35132,7 +35136,7 @@
         <v>46</v>
       </c>
       <c r="I106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -35509,7 +35513,7 @@
         <v>46</v>
       </c>
       <c r="I120" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -35628,7 +35632,7 @@
         <v>46</v>
       </c>
       <c r="I127" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -36005,7 +36009,7 @@
         <v>46</v>
       </c>
       <c r="I141" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -36124,7 +36128,7 @@
         <v>46</v>
       </c>
       <c r="I148" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -36501,7 +36505,7 @@
         <v>46</v>
       </c>
       <c r="I162" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -36620,7 +36624,7 @@
         <v>46</v>
       </c>
       <c r="I169" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -36965,10 +36969,10 @@
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C183" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D183">
         <f>E183/100</f>
@@ -36980,13 +36984,13 @@
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B185" t="s">
         <v>171</v>
       </c>
       <c r="K185" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L185" t="s">
         <v>170</v>
@@ -36994,13 +36998,13 @@
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B187">
         <v>1</v>
       </c>
       <c r="K187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L187">
         <v>10</v>
@@ -37038,13 +37042,13 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>183</v>
+      </c>
+      <c r="B193" t="s">
         <v>184</v>
       </c>
-      <c r="B193" t="s">
-        <v>185</v>
-      </c>
       <c r="K193" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L193" t="s">
         <v>43</v>
@@ -37132,13 +37136,13 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B200" t="s">
         <v>173</v>
       </c>
       <c r="K200" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L200" t="s">
         <v>174</v>
@@ -37146,16 +37150,16 @@
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B202">
         <v>1</v>
       </c>
       <c r="K202" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L202">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
@@ -37169,7 +37173,7 @@
         <v>81</v>
       </c>
       <c r="L204">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.25">
@@ -37185,21 +37189,21 @@
       </c>
       <c r="L206">
         <f>L202+((L204-L202)*$D$183)</f>
-        <v>30</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B208" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K208" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L208" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.25">
@@ -37215,7 +37219,7 @@
       </c>
       <c r="L209">
         <f>ROUND((((1-($K209/5))^2)*L$202)+(2*(1-($K209/5))*($K209/5)*L$206)+((($K209/5)^2)*L$204),0)</f>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.25">
@@ -37231,7 +37235,7 @@
       </c>
       <c r="L210">
         <f>ROUND((((1-($K210/5))^2)*L$202)+(2*(1-($K210/5))*($K210/5)*L$206)+((($K210/5)^2)*L$204),0)</f>
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.25">
@@ -37247,7 +37251,7 @@
       </c>
       <c r="L211">
         <f>ROUND((((1-($K211/5))^2)*L$202)+(2*(1-($K211/5))*($K211/5)*L$206)+((($K211/5)^2)*L$204),0)</f>
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.25">
@@ -37263,7 +37267,7 @@
       </c>
       <c r="L212">
         <f>ROUND((((1-($K212/5))^2)*L$202)+(2*(1-($K212/5))*($K212/5)*L$206)+((($K212/5)^2)*L$204),0)</f>
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.25">
@@ -37279,32 +37283,32 @@
       </c>
       <c r="L213">
         <f>ROUND((((1-($K213/5))^2)*L$202)+(2*(1-($K213/5))*($K213/5)*L$206)+((($K213/5)^2)*L$204),0)</f>
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B215" t="s">
         <v>175</v>
       </c>
       <c r="K215" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L215" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B217">
         <v>0</v>
       </c>
       <c r="K217" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L217">
         <v>4</v>
@@ -37342,13 +37346,13 @@
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B223" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K223" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L223" t="s">
         <v>90</v>
@@ -46272,13 +46276,13 @@
         <v>134</v>
       </c>
       <c r="D2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" t="s">
         <v>189</v>
       </c>
-      <c r="F2" t="s">
-        <v>190</v>
-      </c>
       <c r="H2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J2" t="s">
         <v>136</v>

</xml_diff>